<commit_message>
fix bitmask inspector uses int, add second test item effect
</commit_message>
<xml_diff>
--- a/RoguelikeFNA/Content/translations.xlsx
+++ b/RoguelikeFNA/Content/translations.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="46">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="54">
   <si>
     <t xml:space="preserve">id</t>
   </si>
@@ -158,6 +158,30 @@
   </si>
   <si>
     <t xml:space="preserve">Your projectiles obtain a homing effect.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">regen_item_name</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Regeneracion.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Regen.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">regen_item_desc</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Desc.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">regen_effect_desc</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Regenera {0} vida cada {1} segundos.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Recover {0} health every {1} seconds.</t>
   </si>
 </sst>
 </file>
@@ -468,7 +492,7 @@
   <dimension ref="A1:C20"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C20" activeCellId="0" sqref="C20"/>
+      <selection pane="topLeft" activeCell="C19" activeCellId="0" sqref="C19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.6328125" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -655,9 +679,37 @@
       </c>
     </row>
     <row r="17" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A17" s="0"/>
-      <c r="B17" s="0"/>
-      <c r="C17" s="0"/>
+      <c r="A17" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="B17" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="C17" s="1" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="18" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A18" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="B18" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="C18" s="1" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="19" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A19" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="B19" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="C19" s="1" t="s">
+        <v>53</v>
+      </c>
     </row>
     <row r="20" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C20" s="4"/>

</xml_diff>

<commit_message>
fixes in translation manager and add language on settings
</commit_message>
<xml_diff>
--- a/RoguelikeFNA/Content/translations.xlsx
+++ b/RoguelikeFNA/Content/translations.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="54">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="57">
   <si>
     <t xml:space="preserve">id</t>
   </si>
@@ -182,6 +182,15 @@
   </si>
   <si>
     <t xml:space="preserve">Recover {0} health every {1} seconds.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">language</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Lenguaje</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Language</t>
   </si>
 </sst>
 </file>
@@ -489,10 +498,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:C20"/>
+  <dimension ref="A1:C22"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C19" activeCellId="0" sqref="C19"/>
+      <selection pane="topLeft" activeCell="B15" activeCellId="0" sqref="B15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.6328125" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -712,7 +721,18 @@
       </c>
     </row>
     <row r="20" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C20" s="4"/>
+      <c r="A20" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="B20" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="C20" s="4" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="22" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C22" s="4"/>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>

</xml_diff>

<commit_message>
Essence label translation and essence chase fix
</commit_message>
<xml_diff>
--- a/RoguelikeFNA/Content/translations.xlsx
+++ b/RoguelikeFNA/Content/translations.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="57">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="60">
   <si>
     <t xml:space="preserve">id</t>
   </si>
@@ -191,6 +191,15 @@
   </si>
   <si>
     <t xml:space="preserve">Language</t>
+  </si>
+  <si>
+    <t xml:space="preserve">essence</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Esencia</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Essence</t>
   </si>
 </sst>
 </file>
@@ -501,7 +510,7 @@
   <dimension ref="A1:C22"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B15" activeCellId="0" sqref="B15"/>
+      <selection pane="topLeft" activeCell="C22" activeCellId="0" sqref="C22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.6328125" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -731,6 +740,17 @@
         <v>56</v>
       </c>
     </row>
+    <row r="21" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A21" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="B21" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="C21" s="1" t="s">
+        <v>59</v>
+      </c>
+    </row>
     <row r="22" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C22" s="4"/>
     </row>

</xml_diff>

<commit_message>
refactor stats and new prototype item stat effects
</commit_message>
<xml_diff>
--- a/RoguelikeFNA/Content/translations.xlsx
+++ b/RoguelikeFNA/Content/translations.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="60">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="81" uniqueCount="74">
   <si>
     <t xml:space="preserve">id</t>
   </si>
@@ -200,6 +200,48 @@
   </si>
   <si>
     <t xml:space="preserve">Essence</t>
+  </si>
+  <si>
+    <t xml:space="preserve">dmg_item_name</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Biceps</t>
+  </si>
+  <si>
+    <t xml:space="preserve">dmg_item_desc</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> </t>
+  </si>
+  <si>
+    <t xml:space="preserve">stat_effect_desc</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Incrementa {0} en {1}{2}.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Increments {0} by {1}{2}.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">refstat_effect_desc</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Incrementa tu {0} en {1}{2} de tu {3}.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Increments {0} by {1}{2} of your {3}.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">hptodmg_item_name</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Gigantismo</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Giantism</t>
+  </si>
+  <si>
+    <t xml:space="preserve">hptodmg_item_desc</t>
   </si>
 </sst>
 </file>
@@ -297,7 +339,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="5">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -315,10 +357,6 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -511,10 +549,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:D22"/>
+  <dimension ref="A1:D27"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A10" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C19" activeCellId="0" sqref="C19"/>
+      <selection pane="topLeft" activeCell="A27" activeCellId="0" sqref="A27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.6328125" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -754,10 +792,73 @@
       <c r="C21" s="1" t="s">
         <v>59</v>
       </c>
-      <c r="D21" s="5"/>
+      <c r="D21" s="4"/>
     </row>
     <row r="22" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C22" s="4"/>
+      <c r="A22" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="B22" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="C22" s="1" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="23" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A23" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="B23" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="C23" s="4" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="24" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A24" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="B24" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="C24" s="1" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="25" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A25" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="B25" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="C25" s="1" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="26" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A26" s="3" t="s">
+        <v>70</v>
+      </c>
+      <c r="B26" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="C26" s="1" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="27" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A27" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="B27" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="C27" s="4" t="s">
+        <v>63</v>
+      </c>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>

</xml_diff>